<commit_message>
actualizacion importante y definitiva para S-21 y descarga de los mismos
</commit_message>
<xml_diff>
--- a/Formulario/Informe.xlsx
+++ b/Formulario/Informe.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prueba_info\Sistema actualizado\Sistema-Informes-Google-Appscritp\Formulario\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BFDAA7-8ACF-4A9D-94A7-8A8F534FC73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="form" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="respaldo" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="publicadores" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="clave" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="faltantes" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="inactivos" sheetId="6" r:id="rId9"/>
+    <sheet name="form" sheetId="1" r:id="rId1"/>
+    <sheet name="respaldo" sheetId="2" r:id="rId2"/>
+    <sheet name="publicadores" sheetId="3" r:id="rId3"/>
+    <sheet name="clave" sheetId="4" r:id="rId4"/>
+    <sheet name="faltantes" sheetId="5" r:id="rId5"/>
+    <sheet name="inactivos" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>nombre</t>
   </si>
@@ -56,26 +65,62 @@
   <si>
     <t>fecha</t>
   </si>
+  <si>
+    <t>fecha_n</t>
+  </si>
+  <si>
+    <t>fecha_b</t>
+  </si>
+  <si>
+    <t>sexo</t>
+  </si>
+  <si>
+    <t>condicion</t>
+  </si>
+  <si>
+    <t>siervo</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>anciano</t>
+  </si>
+  <si>
+    <t>especial</t>
+  </si>
+  <si>
+    <t>misionero</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,11 +128,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="4">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -98,55 +149,72 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -336,20 +404,23 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -379,21 +450,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,113 +495,147 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregado de actualizaciones tanto los documentos y la logica
</commit_message>
<xml_diff>
--- a/Formulario/Informe.xlsx
+++ b/Formulario/Informe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prueba_info\Sistema actualizado\Sistema-Informes-Google-Appscritp\Formulario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Actualizacion sistema\Sistema-Informes-Google-Appscritp\Formulario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BFDAA7-8ACF-4A9D-94A7-8A8F534FC73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD61F29C-5D6C-4820-9D67-693FBE0AC678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="form" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,13 @@
     <sheet name="publicadores" sheetId="3" r:id="rId3"/>
     <sheet name="clave" sheetId="4" r:id="rId4"/>
     <sheet name="faltantes" sheetId="5" r:id="rId5"/>
-    <sheet name="inactivos" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>nombre</t>
   </si>
@@ -61,9 +60,6 @@
   </si>
   <si>
     <t>contrasena</t>
-  </si>
-  <si>
-    <t>fecha</t>
   </si>
   <si>
     <t>fecha_n</t>
@@ -416,7 +412,7 @@
   </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -526,31 +522,31 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>7</v>
@@ -608,34 +604,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>